<commit_message>
added color coding to outputs, formatting, added other models' columns
</commit_message>
<xml_diff>
--- a/best_model_performance.xlsx
+++ b/best_model_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ARSH\NEU\Fall 2021\CS 5100\Projects\NIH_Disease_Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DA3B82A-496A-4DC9-9C93-556153777FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4544537-6689-45C9-AB4A-68A831F9BF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9024DD29-FBB4-4EC1-9DE5-C3D906D15B79}"/>
+    <workbookView xWindow="-28920" yWindow="-3495" windowWidth="29040" windowHeight="17640" xr2:uid="{9024DD29-FBB4-4EC1-9DE5-C3D906D15B79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Disease</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>Average for All Diseases</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>GaussianNB</t>
+  </si>
+  <si>
+    <t>BernoulliNB</t>
+  </si>
+  <si>
+    <t>Decision Trees</t>
   </si>
 </sst>
 </file>
@@ -110,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,16 +138,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -143,11 +192,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -156,11 +257,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="3" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -472,90 +589,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF02A92-64A2-4C0A-9567-A021B4B6CBC2}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:D6"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" customWidth="1"/>
+    <col min="17" max="17" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="K3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="L3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="M3" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="N3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -567,18 +738,18 @@
       <c r="D6">
         <v>0.76700000000000002</v>
       </c>
-      <c r="F6">
+      <c r="J6">
         <v>0.76400000000000001</v>
       </c>
-      <c r="G6">
+      <c r="K6">
         <v>0.76700000000000002</v>
       </c>
-      <c r="H6">
+      <c r="L6">
         <v>0.755</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -590,18 +761,18 @@
       <c r="D7">
         <v>0.749</v>
       </c>
-      <c r="F7">
+      <c r="J7">
         <v>0.66900000000000004</v>
       </c>
-      <c r="G7">
+      <c r="K7">
         <v>0.76600000000000001</v>
       </c>
-      <c r="H7">
+      <c r="L7">
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -613,18 +784,18 @@
       <c r="D8">
         <v>0.73799999999999999</v>
       </c>
-      <c r="F8">
+      <c r="J8">
         <v>0.75</v>
       </c>
-      <c r="G8">
+      <c r="K8">
         <v>0.70599999999999996</v>
       </c>
-      <c r="H8">
+      <c r="L8">
         <v>0.73099999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -636,18 +807,18 @@
       <c r="D9">
         <v>0.86</v>
       </c>
-      <c r="F9">
+      <c r="J9">
         <v>0.85699999999999998</v>
       </c>
-      <c r="G9">
+      <c r="K9">
         <v>0.89200000000000002</v>
       </c>
-      <c r="H9">
+      <c r="L9">
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -659,18 +830,18 @@
       <c r="D10">
         <v>0.76700000000000002</v>
       </c>
-      <c r="F10">
+      <c r="J10">
         <v>0.749</v>
       </c>
-      <c r="G10">
+      <c r="K10">
         <v>0.78100000000000003</v>
       </c>
-      <c r="H10">
+      <c r="L10">
         <v>0.73599999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -682,18 +853,18 @@
       <c r="D11">
         <v>0.80500000000000005</v>
       </c>
-      <c r="F11">
+      <c r="J11">
         <v>0.75700000000000001</v>
       </c>
-      <c r="G11">
+      <c r="K11">
         <v>0.85399999999999998</v>
       </c>
-      <c r="H11">
+      <c r="L11">
         <v>0.751</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -705,18 +876,18 @@
       <c r="D12">
         <v>0.83499999999999996</v>
       </c>
-      <c r="F12">
+      <c r="J12">
         <v>0.84499999999999997</v>
       </c>
-      <c r="G12">
+      <c r="K12">
         <v>0.80500000000000005</v>
       </c>
-      <c r="H12">
+      <c r="L12">
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -728,18 +899,18 @@
       <c r="D13">
         <v>0.99299999999999999</v>
       </c>
-      <c r="F13">
+      <c r="J13">
         <v>0.88300000000000001</v>
       </c>
-      <c r="G13">
+      <c r="K13">
         <v>0.70499999999999996</v>
       </c>
-      <c r="H13">
+      <c r="L13">
         <v>0.996</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -751,18 +922,18 @@
       <c r="D14">
         <v>0.67700000000000005</v>
       </c>
-      <c r="F14">
+      <c r="J14">
         <v>0.68200000000000005</v>
       </c>
-      <c r="G14">
+      <c r="K14">
         <v>0.68300000000000005</v>
       </c>
-      <c r="H14">
+      <c r="L14">
         <v>0.68799999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -774,18 +945,18 @@
       <c r="D15">
         <v>0.68899999999999995</v>
       </c>
-      <c r="F15">
+      <c r="J15">
         <v>0.67300000000000004</v>
       </c>
-      <c r="G15">
+      <c r="K15">
         <v>0.68700000000000006</v>
       </c>
-      <c r="H15">
+      <c r="L15">
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -797,18 +968,18 @@
       <c r="D16">
         <v>0.68700000000000006</v>
       </c>
-      <c r="F16">
+      <c r="J16">
         <v>0.68300000000000005</v>
       </c>
-      <c r="G16">
+      <c r="K16">
         <v>0.71499999999999997</v>
       </c>
-      <c r="H16">
+      <c r="L16">
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -820,18 +991,18 @@
       <c r="D17">
         <v>0.71899999999999997</v>
       </c>
-      <c r="F17">
+      <c r="J17">
         <v>0.73199999999999998</v>
       </c>
-      <c r="G17">
+      <c r="K17">
         <v>0.745</v>
       </c>
-      <c r="H17">
+      <c r="L17">
         <v>0.73199999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -843,18 +1014,18 @@
       <c r="D18">
         <v>0.69399999999999995</v>
       </c>
-      <c r="F18">
+      <c r="J18">
         <v>0.66100000000000003</v>
       </c>
-      <c r="G18">
+      <c r="K18">
         <v>0.79400000000000004</v>
       </c>
-      <c r="H18">
+      <c r="L18">
         <v>0.75700000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -866,59 +1037,411 @@
       <c r="D19">
         <v>0.77500000000000002</v>
       </c>
-      <c r="F19">
+      <c r="J19">
         <v>0.73599999999999999</v>
       </c>
-      <c r="G19">
+      <c r="K19">
         <v>0.747</v>
       </c>
-      <c r="H19">
+      <c r="L19">
         <v>0.77600000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <f>AVERAGE(B6:B19)</f>
         <v>0.74564285714285694</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <f>AVERAGE(C6:C19)</f>
         <v>0.75542857142857134</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <f>AVERAGE(D6:D19)</f>
         <v>0.76821428571428574</v>
       </c>
-      <c r="E21" s="5" t="e">
-        <f t="shared" ref="C21:I21" si="0">AVERAGE(E6:E19)</f>
+      <c r="E21" s="4" t="e">
+        <f t="shared" ref="E21:M21" si="0">AVERAGE(E6:E19)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F21" s="5">
-        <f>AVERAGE(F6:F19)</f>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4">
+        <f>AVERAGE(J6:J19)</f>
         <v>0.74578571428571439</v>
       </c>
-      <c r="G21" s="5">
+      <c r="K21" s="4">
         <f t="shared" si="0"/>
         <v>0.76050000000000006</v>
       </c>
-      <c r="H21" s="5">
+      <c r="L21" s="4">
         <f t="shared" si="0"/>
         <v>0.76928571428571413</v>
       </c>
-      <c r="I21" s="5" t="e">
+      <c r="M21" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B6:I6">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:I7">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:I8">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:I9">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:I10">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:I11">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:I12">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:I13">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:I14">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:I15">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:I16">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:I17">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:I18">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:I19">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6:Q6">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:Q7">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8:Q8">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:Q9">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:Q10">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:Q11">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12:Q12">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13:Q13">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14:Q14">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:Q15">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16:Q16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17:Q17">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18:Q18">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19:Q19">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:Q21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added results of ML models with CNN features
</commit_message>
<xml_diff>
--- a/best_model_performance.xlsx
+++ b/best_model_performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ARSH\NEU\Fall 2021\CS 5100\Projects\NIH_Disease_Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4544537-6689-45C9-AB4A-68A831F9BF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF6BC3B-1834-4581-A81A-19792A5DC0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3495" windowWidth="29040" windowHeight="17640" xr2:uid="{9024DD29-FBB4-4EC1-9DE5-C3D906D15B79}"/>
   </bookViews>
@@ -248,7 +248,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -264,13 +264,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -589,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF02A92-64A2-4C0A-9567-A021B4B6CBC2}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,38 +610,40 @@
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
     <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.109375" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" customWidth="1"/>
-    <col min="17" max="17" width="8.77734375" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" customWidth="1"/>
+    <col min="14" max="14" width="7.44140625" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" customWidth="1"/>
+    <col min="18" max="18" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -646,11 +652,12 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="2"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:17" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
@@ -675,58 +682,59 @@
       <c r="I3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -738,18 +746,42 @@
       <c r="D6">
         <v>0.76700000000000002</v>
       </c>
-      <c r="J6">
+      <c r="F6" s="11">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="K6">
         <v>0.76400000000000001</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.76700000000000002</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>0.755</v>
       </c>
+      <c r="O6">
+        <v>0.78</v>
+      </c>
+      <c r="P6">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="Q6">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="R6">
+        <v>0.52200000000000002</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -761,18 +793,42 @@
       <c r="D7">
         <v>0.749</v>
       </c>
-      <c r="J7">
+      <c r="F7" s="11">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7">
         <v>0.66900000000000004</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.76600000000000001</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0.78300000000000003</v>
       </c>
+      <c r="O7">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="P7">
+        <v>0.503</v>
+      </c>
+      <c r="Q7">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="R7">
+        <v>0.501</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -784,18 +840,42 @@
       <c r="D8">
         <v>0.73799999999999999</v>
       </c>
-      <c r="J8">
+      <c r="F8" s="11">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8">
         <v>0.75</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>0.70599999999999996</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>0.73099999999999998</v>
       </c>
+      <c r="O8">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="P8">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="Q8">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="R8">
+        <v>0.503</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -807,18 +887,42 @@
       <c r="D9">
         <v>0.86</v>
       </c>
-      <c r="J9">
+      <c r="F9" s="11">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="K9">
         <v>0.85699999999999998</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0.89200000000000002</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>0.85699999999999998</v>
       </c>
+      <c r="O9">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="P9">
+        <v>0.77</v>
+      </c>
+      <c r="Q9">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="R9">
+        <v>0.501</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -830,18 +934,42 @@
       <c r="D10">
         <v>0.76700000000000002</v>
       </c>
-      <c r="J10">
+      <c r="F10" s="11">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0.72</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="K10">
         <v>0.749</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0.78100000000000003</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>0.73599999999999999</v>
       </c>
+      <c r="O10">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="P10">
+        <v>0.68</v>
+      </c>
+      <c r="Q10">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="R10">
+        <v>0.52800000000000002</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -853,18 +981,42 @@
       <c r="D11">
         <v>0.80500000000000005</v>
       </c>
-      <c r="J11">
+      <c r="F11" s="11">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="K11">
         <v>0.75700000000000001</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>0.85399999999999998</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0.751</v>
       </c>
+      <c r="O11">
+        <v>0.8</v>
+      </c>
+      <c r="P11">
+        <v>0.625</v>
+      </c>
+      <c r="Q11">
+        <v>0.755</v>
+      </c>
+      <c r="R11">
+        <v>0.52300000000000002</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -876,18 +1028,42 @@
       <c r="D12">
         <v>0.83499999999999996</v>
       </c>
-      <c r="J12">
+      <c r="F12" s="11">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="K12">
         <v>0.84499999999999997</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.80500000000000005</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>0.84599999999999997</v>
       </c>
+      <c r="O12">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="P12">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="Q12">
+        <v>0.755</v>
+      </c>
+      <c r="R12">
+        <v>0.49</v>
+      </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -899,18 +1075,42 @@
       <c r="D13">
         <v>0.99299999999999999</v>
       </c>
-      <c r="J13">
+      <c r="F13" s="11">
+        <v>0.998</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="K13">
         <v>0.88300000000000001</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0.70499999999999996</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.996</v>
       </c>
+      <c r="O13">
+        <v>0.622</v>
+      </c>
+      <c r="P13">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="Q13">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="R13">
+        <v>0.498</v>
+      </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -922,18 +1122,42 @@
       <c r="D14">
         <v>0.67700000000000005</v>
       </c>
-      <c r="J14">
+      <c r="F14" s="11">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0.626</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="K14">
         <v>0.68200000000000005</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0.68300000000000005</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>0.68799999999999994</v>
       </c>
+      <c r="O14">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="P14">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="Q14">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="R14">
+        <v>0.53500000000000003</v>
+      </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -945,18 +1169,42 @@
       <c r="D15">
         <v>0.68899999999999995</v>
       </c>
-      <c r="J15">
+      <c r="F15" s="11">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="K15">
         <v>0.67300000000000004</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>0.68700000000000006</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>0.66700000000000004</v>
       </c>
+      <c r="O15">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="P15">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="Q15">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="R15">
+        <v>0.53800000000000003</v>
+      </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -968,18 +1216,42 @@
       <c r="D16">
         <v>0.68700000000000006</v>
       </c>
-      <c r="J16">
+      <c r="F16" s="11">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0.62</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="K16">
         <v>0.68300000000000005</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>0.71499999999999997</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>0.69499999999999995</v>
       </c>
+      <c r="O16">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="P16">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="Q16">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="R16">
+        <v>0.51700000000000002</v>
+      </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -991,18 +1263,42 @@
       <c r="D17">
         <v>0.71899999999999997</v>
       </c>
-      <c r="J17">
+      <c r="F17" s="11">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="K17">
         <v>0.73199999999999998</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>0.745</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>0.73199999999999998</v>
       </c>
+      <c r="O17">
+        <v>0.749</v>
+      </c>
+      <c r="P17">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="Q17">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="R17">
+        <v>0.50600000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -1014,18 +1310,42 @@
       <c r="D18">
         <v>0.69399999999999995</v>
       </c>
-      <c r="J18">
+      <c r="F18" s="11">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="K18">
         <v>0.66100000000000003</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>0.79400000000000004</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>0.75700000000000001</v>
       </c>
+      <c r="O18">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P18">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="Q18">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="R18">
+        <v>0.49299999999999999</v>
+      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -1037,18 +1357,42 @@
       <c r="D19">
         <v>0.77500000000000002</v>
       </c>
-      <c r="J19">
+      <c r="F19" s="11">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="G19" s="11">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="H19" s="11">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="K19">
         <v>0.73599999999999999</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>0.747</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>0.77600000000000002</v>
       </c>
+      <c r="O19">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="P19">
+        <v>0.66</v>
+      </c>
+      <c r="Q19">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="R19">
+        <v>0.54700000000000004</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="4">
@@ -1064,37 +1408,66 @@
         <v>0.76821428571428574</v>
       </c>
       <c r="E21" s="4" t="e">
-        <f t="shared" ref="E21:M21" si="0">AVERAGE(E6:E19)</f>
+        <f t="shared" ref="E21:R21" si="0">AVERAGE(E6:E19)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4">
-        <f>AVERAGE(J6:J19)</f>
+      <c r="F21" s="4">
+        <f>AVERAGE(F6:F19)</f>
+        <v>0.83114285714285718</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" ref="G21:I21" si="1">AVERAGE(G6:G19)</f>
+        <v>0.68071428571428583</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="1"/>
+        <v>0.69478571428571434</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4">
+        <f>AVERAGE(K6:K19)</f>
         <v>0.74578571428571439</v>
       </c>
-      <c r="K21" s="4">
+      <c r="L21" s="4">
         <f t="shared" si="0"/>
         <v>0.76050000000000006</v>
       </c>
-      <c r="L21" s="4">
+      <c r="M21" s="4">
         <f t="shared" si="0"/>
         <v>0.76928571428571413</v>
       </c>
-      <c r="M21" s="4" t="e">
+      <c r="N21" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="0"/>
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="P21" s="4">
+        <f t="shared" si="0"/>
+        <v>0.64914285714285724</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="0"/>
+        <v>0.69192857142857134</v>
+      </c>
+      <c r="R21" s="4">
+        <f t="shared" si="0"/>
+        <v>0.51442857142857157</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6:I6">
+  <conditionalFormatting sqref="B6:J6 I7:J19">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -1106,7 +1479,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:I7">
+  <conditionalFormatting sqref="B7:H7">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -1118,7 +1491,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:I8">
+  <conditionalFormatting sqref="B8:H8">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -1130,7 +1503,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:I9">
+  <conditionalFormatting sqref="B9:H9">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -1142,7 +1515,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:I10">
+  <conditionalFormatting sqref="B10:H10">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -1154,7 +1527,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:I11">
+  <conditionalFormatting sqref="B11:H11">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -1166,7 +1539,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:I12">
+  <conditionalFormatting sqref="B12:H12">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -1178,7 +1551,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:I13">
+  <conditionalFormatting sqref="B13:H13">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -1190,7 +1563,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:I14">
+  <conditionalFormatting sqref="B14:H14">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -1202,7 +1575,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:I15">
+  <conditionalFormatting sqref="B15:H15">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -1214,7 +1587,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:I16">
+  <conditionalFormatting sqref="B16:H16">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -1226,7 +1599,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:I17">
+  <conditionalFormatting sqref="B17:H17">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -1238,7 +1611,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:I18">
+  <conditionalFormatting sqref="B18:H18">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -1250,7 +1623,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:I19">
+  <conditionalFormatting sqref="B19:H19">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -1262,7 +1635,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6:Q6">
+  <conditionalFormatting sqref="K6:R6">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -1274,7 +1647,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:Q7">
+  <conditionalFormatting sqref="K7:R7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -1286,7 +1659,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J8:Q8">
+  <conditionalFormatting sqref="K8:R8">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -1298,7 +1671,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9:Q9">
+  <conditionalFormatting sqref="K9:R9">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -1310,7 +1683,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10:Q10">
+  <conditionalFormatting sqref="K10:Q10 R10:R11">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -1322,7 +1695,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:Q11">
+  <conditionalFormatting sqref="K11:Q11 R12">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -1334,7 +1707,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J12:Q12">
+  <conditionalFormatting sqref="K12:Q12 R13">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -1346,7 +1719,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13:Q13">
+  <conditionalFormatting sqref="K13:Q13 R14">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1358,7 +1731,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14:Q14">
+  <conditionalFormatting sqref="K14:Q14 R15">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1370,7 +1743,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J15:Q15">
+  <conditionalFormatting sqref="K15:Q15 R16">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1382,7 +1755,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J16:Q16">
+  <conditionalFormatting sqref="K16:Q16 R17">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1394,7 +1767,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J17:Q17">
+  <conditionalFormatting sqref="K17:Q17 R18">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1406,7 +1779,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J18:Q18">
+  <conditionalFormatting sqref="K18:Q18 R19">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1418,7 +1791,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J19:Q19">
+  <conditionalFormatting sqref="K19:Q19">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1430,7 +1803,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:Q21">
+  <conditionalFormatting sqref="B21:R21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>